<commit_message>
test pushing without pulling
</commit_message>
<xml_diff>
--- a/ChoosingParameters/simTimeNoPred.xlsx
+++ b/ChoosingParameters/simTimeNoPred.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>pop</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>total min (h)</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>maxCons</t>
+  </si>
+  <si>
+    <t>sizeEq</t>
   </si>
 </sst>
 </file>
@@ -91,8 +100,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -100,9 +119,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,141 +461,558 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="7" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>75000</v>
+      </c>
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>280</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>290</v>
       </c>
-      <c r="E2">
-        <f>C2*$B2</f>
+      <c r="H2">
+        <f>F2*$E2</f>
         <v>840</v>
       </c>
-      <c r="F2">
-        <f>D2*$B2</f>
+      <c r="I2">
+        <f>G2*$E2</f>
         <v>870</v>
       </c>
-      <c r="G2" s="1">
-        <f>E2/3600</f>
+      <c r="J2" s="1">
+        <f>H2/3600</f>
         <v>0.23333333333333334</v>
       </c>
-      <c r="H2" s="1">
-        <f>F2/3600</f>
+      <c r="K2" s="1">
+        <f>I2/3600</f>
         <v>0.24166666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>100</v>
       </c>
       <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>75000</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>410</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>413</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:F4" si="0">C3*$B3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:I4" si="0">F3*$E3</f>
         <v>1230</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <f t="shared" si="0"/>
         <v>1239</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:H4" si="1">E3/3600</f>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:K4" si="1">H3/3600</f>
         <v>0.34166666666666667</v>
       </c>
-      <c r="H3" s="1">
+      <c r="K3" s="1">
         <f t="shared" si="1"/>
         <v>0.34416666666666668</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1000</v>
       </c>
       <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>75000</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="F4">
         <v>522</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>527</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>1566</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>1581</v>
       </c>
-      <c r="G4" s="1">
+      <c r="J4" s="1">
         <f t="shared" si="1"/>
         <v>0.435</v>
       </c>
-      <c r="H4" s="1">
+      <c r="K4" s="1">
         <f t="shared" si="1"/>
         <v>0.43916666666666665</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="G5" s="1">
-        <f>SUM(G2:G4)</f>
+    <row r="5" spans="1:11">
+      <c r="J5" s="1">
+        <f>SUM(J2:J4)</f>
         <v>1.01</v>
       </c>
-      <c r="H5" s="1">
-        <f>SUM(H2:H4)</f>
+      <c r="K5" s="1">
+        <f>SUM(K2:K4)</f>
         <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>38000</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>157</v>
+      </c>
+      <c r="G6">
+        <v>168</v>
+      </c>
+      <c r="H6">
+        <f>F6*$E6</f>
+        <v>1570</v>
+      </c>
+      <c r="I6">
+        <f>G6*$E6</f>
+        <v>1680</v>
+      </c>
+      <c r="J6" s="1">
+        <f>H6/3600</f>
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="K6" s="1">
+        <f>I6/3600</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>38000</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>224</v>
+      </c>
+      <c r="G7">
+        <v>228</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H8" si="2">F7*$E7</f>
+        <v>2240</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I8" si="3">G7*$E7</f>
+        <v>2280</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" ref="J7:J8" si="4">H7/3600</f>
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7:K8" si="5">I7/3600</f>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>38000</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>285</v>
+      </c>
+      <c r="G8">
+        <v>293</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>2850</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>2930</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="4"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="5"/>
+        <v>0.81388888888888888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="J9" s="1">
+        <f>SUM(J6:J8)</f>
+        <v>1.85</v>
+      </c>
+      <c r="K9" s="1">
+        <f>SUM(K6:K8)</f>
+        <v>1.913888888888889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4400</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <f>F10*$E10</f>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f>G10*$E10</f>
+        <v>20</v>
+      </c>
+      <c r="J10" s="1">
+        <f>H10/3600</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10/3600</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4400</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H12" si="6">F11*$E11</f>
+        <v>20</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I12" si="7">G11*$E11</f>
+        <v>20</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" ref="J11:J12" si="8">H11/3600</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" ref="K11:K12" si="9">I11/3600</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>4400</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="8"/>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="9"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="J13" s="1">
+        <f>SUM(J10:J12)</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <f>SUM(K10:K12)</f>
+        <v>1.9444444444444445E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>2300</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f>F14*$E14</f>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f>G14*$E14</f>
+        <v>10</v>
+      </c>
+      <c r="J14" s="1">
+        <f>H14/3600</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14/3600</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>2300</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:H16" si="10">F15*$E15</f>
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I16" si="11">G15*$E15</f>
+        <v>10</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" ref="J15:J16" si="12">H15/3600</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" ref="K15:K16" si="13">I15/3600</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>2300</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="12"/>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="13"/>
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11">
+      <c r="J17" s="1">
+        <f>SUM(J14:J16)</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="K17" s="1">
+        <f>SUM(K14:K16)</f>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>